<commit_message>
Add functionality to generate synthetic survey records and compare distributions
</commit_message>
<xml_diff>
--- a/Encuestas/IE.2025.treated.xlsx
+++ b/Encuestas/IE.2025.treated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\70254057\Desktop\basic-hub\LocalWealthHousing\Encuestas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF888E5-5B85-450D-9F7F-7CD6DA690466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C01B4D5-D6FE-4922-9E8B-4381BE3E1A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{AFC643AB-D246-47A2-A017-5711B6631554}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{AFC643AB-D246-47A2-A017-5711B6631554}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2844" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2843" uniqueCount="296">
   <si>
     <t>Id</t>
   </si>
@@ -1319,14 +1319,14 @@
       <selection activeCell="F16" sqref="A1:W50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" customWidth="1"/>
     <col min="13" max="13" width="12" customWidth="1"/>
-    <col min="17" max="17" width="20.140625" customWidth="1"/>
+    <col min="17" max="17" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2860,7 +2860,7 @@
       </c>
       <c r="X24" s="1"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -3186,7 +3186,7 @@
       </c>
       <c r="X29" s="1"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -3315,7 +3315,7 @@
       <c r="X31" s="1"/>
       <c r="Y31" s="1"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3445,7 +3445,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3921,7 +3921,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4119,7 +4119,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4187,7 +4187,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4323,7 +4323,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4391,7 +4391,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4459,7 +4459,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4527,7 +4527,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4601,22 +4601,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C843C03-1659-4A64-A5A7-311B5EB269A9}">
   <dimension ref="A1:W57"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N35" sqref="A1:W57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" customWidth="1"/>
     <col min="11" max="11" width="24" customWidth="1"/>
-    <col min="13" max="13" width="23.5703125" customWidth="1"/>
-    <col min="16" max="16" width="28.5703125" customWidth="1"/>
-    <col min="17" max="17" width="22.42578125" style="3" customWidth="1"/>
-    <col min="22" max="22" width="27.42578125" customWidth="1"/>
+    <col min="13" max="13" width="23.5546875" customWidth="1"/>
+    <col min="16" max="16" width="28.5546875" customWidth="1"/>
+    <col min="17" max="17" width="22.44140625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4687,7 +4687,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4814,7 +4814,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4882,7 +4882,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4950,7 +4950,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5015,7 +5015,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5080,7 +5080,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5145,7 +5145,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5213,7 +5213,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5411,7 +5411,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5476,7 +5476,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5544,7 +5544,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5664,7 +5664,7 @@
       </c>
       <c r="W16" s="1"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5726,7 +5726,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5782,7 +5782,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5844,7 +5844,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5909,7 +5909,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5959,7 +5959,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="22" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -6024,7 +6024,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -6086,7 +6086,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -6130,7 +6130,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -6195,7 +6195,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -6260,7 +6260,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -6321,7 +6321,7 @@
       </c>
       <c r="W27" s="1"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -6382,7 +6382,7 @@
       </c>
       <c r="W28" s="1"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -6441,7 +6441,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -6509,7 +6509,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -6577,7 +6577,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -6645,7 +6645,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -6710,7 +6710,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -6757,7 +6757,7 @@
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -6819,7 +6819,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -6879,7 +6879,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -6939,7 +6939,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -7004,7 +7004,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -7069,7 +7069,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -7134,7 +7134,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -7202,7 +7202,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -7270,7 +7270,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -7338,7 +7338,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -7406,7 +7406,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -7474,7 +7474,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -7542,7 +7542,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -7610,7 +7610,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -7672,7 +7672,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -7740,7 +7740,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -7808,7 +7808,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -7876,7 +7876,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -7944,7 +7944,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -8012,7 +8012,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -8080,7 +8080,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -8148,7 +8148,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -8216,7 +8216,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -8290,17 +8290,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71866E45-EB0F-4F78-ACCA-99A6D4CA7E36}">
   <dimension ref="A1:W57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="8" max="8" width="50.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="50.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="62.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="82" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8371,7 +8388,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -8433,7 +8450,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -8498,7 +8515,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -8566,7 +8583,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -8634,7 +8651,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -8699,7 +8716,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -8764,7 +8781,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -8829,7 +8846,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -8897,7 +8914,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -8959,7 +8976,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -9027,7 +9044,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -9095,7 +9112,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -9160,7 +9177,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -9228,7 +9245,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -9293,10 +9310,19 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
+      <c r="B16">
+        <v>45645.428923611114</v>
+      </c>
+      <c r="C16">
+        <v>45645.437094907407</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
       <c r="F16" s="2">
         <v>20</v>
       </c>
@@ -9337,7 +9363,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -9399,7 +9425,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -9412,8 +9438,8 @@
       <c r="D18" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>122</v>
+      <c r="F18" s="2">
+        <v>18</v>
       </c>
       <c r="G18" t="s">
         <v>123</v>
@@ -9455,7 +9481,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -9517,7 +9543,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -9582,7 +9608,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -9632,7 +9658,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -9697,7 +9723,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -9759,7 +9785,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -9803,7 +9829,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -9868,7 +9894,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -9930,7 +9956,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -9986,7 +10012,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -10042,7 +10068,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -10101,7 +10127,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -10169,7 +10195,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -10237,7 +10263,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -10305,7 +10331,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -10367,7 +10393,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -10402,7 +10428,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -10464,7 +10490,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -10523,7 +10549,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -10582,7 +10608,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -10595,8 +10621,8 @@
       <c r="D38" t="s">
         <v>23</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>219</v>
+      <c r="F38" s="2">
+        <v>18</v>
       </c>
       <c r="G38" t="s">
         <v>55</v>
@@ -10644,7 +10670,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -10709,7 +10735,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -10774,7 +10800,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -10842,7 +10868,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -10910,7 +10936,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -10978,7 +11004,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -11046,7 +11072,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -11114,7 +11140,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -11182,7 +11208,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -11250,7 +11276,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -11312,7 +11338,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -11380,7 +11406,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -11448,7 +11474,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -11516,7 +11542,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -11584,7 +11610,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -11652,7 +11678,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -11720,7 +11746,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -11788,7 +11814,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -11856,7 +11882,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>

</xml_diff>